<commit_message>
read excel file and sort data
</commit_message>
<xml_diff>
--- a/app/assets/uploads/invoicing_party.xlsx
+++ b/app/assets/uploads/invoicing_party.xlsx
@@ -233,7 +233,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -338,7 +338,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>134.2654</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>